<commit_message>
Stuff I forgot to commit earlier
</commit_message>
<xml_diff>
--- a/Interference Calcs.xlsx
+++ b/Interference Calcs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlosj\Documents\FRC\flywheel-design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRC\Flywheel-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21347FA-BD60-42F7-94E5-E82E0583762E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Pressure</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Hub</t>
   </si>
   <si>
-    <t>kb</t>
-  </si>
-  <si>
     <t>kh</t>
   </si>
   <si>
@@ -96,12 +94,27 @@
   </si>
   <si>
     <t>in</t>
+  </si>
+  <si>
+    <t>Clearance needed</t>
+  </si>
+  <si>
+    <t>Max bronze-steel interference</t>
+  </si>
+  <si>
+    <t>Max hub-bronze interference</t>
+  </si>
+  <si>
+    <t>kbs</t>
+  </si>
+  <si>
+    <t>ks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -165,12 +178,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -451,24 +464,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -478,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -519,23 +533,23 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="5"/>
       <c r="F8">
-        <v>2E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="G8">
         <f>F8/((1/C4)+(1/C11))</f>
-        <v>199.60079840319361</v>
+        <v>349.30139720558878</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -546,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -597,158 +611,255 @@
         <v>107526.88172043012</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="G15">
+        <f>F15/((1/C11)+(1/C17))</f>
+        <v>308.98256455528576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" t="e">
+        <f t="shared" ref="C16:C18" si="1">A16/B16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>200</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4.0549999999999999E-4</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>493218.24907521578</v>
+      </c>
+    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="A18">
+        <v>500</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0139999999999999E-3</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>493096.64694280084</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2">
         <v>300</v>
       </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C28" t="s">
         <v>8</v>
-      </c>
-      <c r="B19" s="3">
-        <v>-320</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <f>B18-B20</f>
-        <v>225</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <f>B19-B20</f>
-        <v>-395</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="3">
-        <v>3.875</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1.2999999999999999E-5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1.0200000000000001E-5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="4">
-        <v>5.9000000000000003E-6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="5">
-        <f>B24+(B24*B27*B21)</f>
-        <v>3.8801440624999999</v>
+        <v>7</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-320</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="5">
-        <f>B24+(B24*B26*B22)</f>
-        <v>3.8593876250000001</v>
+        <v>19</v>
+      </c>
+      <c r="B30" s="2">
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="5">
-        <f>B23+(B23*B26*B21)</f>
-        <v>3.5080325000000001</v>
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <f>B28-B30</f>
+        <v>225</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <f>B29-B30</f>
+        <v>-395</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3.875</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="C35" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="5">
-        <f>B23+(B23*B25*B22)</f>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1.0200000000000001E-5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3">
+        <v>5.9000000000000003E-6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="4">
+        <f>B34+(B34*B37*B31)</f>
+        <v>3.8801440624999999</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="4">
+        <f>B34+(B34*B36*B32)</f>
+        <v>3.8593876250000001</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B33+(B33*B36*B31)</f>
+        <v>3.5080325000000001</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B33+(B33*B35*B32)</f>
         <v>3.4820275000000001</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="4">
+        <f>(B39-B40)-B43</f>
+        <v>1.9756437499999779E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="4">
+        <f>(B41-B42)-B43</f>
+        <v>2.5005000000000055E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>